<commit_message>
Minor changes in what transcript is initially displayed. Switched to highgest scoring.
</commit_message>
<xml_diff>
--- a/paper/data/published-variants-for-simulation_2021-01-22.xlsx
+++ b/paper/data/published-variants-for-simulation_2021-01-22.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6D4AAD-5DE6-0E4B-9018-B8DE5BA81DF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E320F28-C3AE-084A-A6F7-FFB711961303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="500" windowWidth="67740" windowHeight="27240" activeTab="1" xr2:uid="{AE07EF24-9AED-F04B-83D6-329CC7A00702}"/>
+    <workbookView xWindow="-20" yWindow="520" windowWidth="28800" windowHeight="16780" activeTab="1" xr2:uid="{AE07EF24-9AED-F04B-83D6-329CC7A00702}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -2176,7 +2176,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3410,7 +3410,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>304</v>
       </c>

</xml_diff>